<commit_message>
Commited save reserved seat, and disable reserved seat feature
</commit_message>
<xml_diff>
--- a/Session1/marking.xlsx
+++ b/Session1/marking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Latihan C#\BNSC\BNSC2017\Soal\session1\session1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Latihan C#\BNSC2017 Review\Session1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -114,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -169,10 +175,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,13 +515,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>8</v>
       </c>
       <c r="D2">
@@ -523,130 +530,130 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="7">
         <v>5</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="7">
         <v>8</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="7">
         <v>8</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="7">
         <v>5</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="7">
         <v>8</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="7">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
@@ -655,20 +662,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="7">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commited print to textfile function
</commit_message>
<xml_diff>
--- a/Session1/marking.xlsx
+++ b/Session1/marking.xlsx
@@ -490,7 +490,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +646,7 @@
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="7">
         <v>9</v>
       </c>
     </row>

</xml_diff>